<commit_message>
07/03/24 Actualización de preventivos 2023-2024
</commit_message>
<xml_diff>
--- a/Locations.xlsx
+++ b/Locations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lperez\Desktop\dash\dash-tecnonorte\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lperez\Desktop\dash-tecnonorte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A877CF8-9135-4721-BB8C-3547096CA8E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1961E248-A1A1-45A2-B5F4-EFB8FF19E5A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Locations" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,17 @@
     <definedName name="ClientesLista">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1489,7 +1500,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1503,8 +1514,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1862,8 +1871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3332,16 +3341,16 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A105" s="9" t="s">
+      <c r="A105" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B105" s="9" t="s">
+      <c r="B105" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C105" s="10" t="s">
+      <c r="C105" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="D105" s="10" t="s">
+      <c r="D105" s="7" t="s">
         <v>183</v>
       </c>
     </row>

</xml_diff>